<commit_message>
added a ton of photos
</commit_message>
<xml_diff>
--- a/gpuSpec.xlsx
+++ b/gpuSpec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/636e7371d64a1ee5/source tree/1west-mec/Shopping-Cart-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\OneDrive\source tree\1west-mec\Shopping-Cart-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
   <si>
     <t>Gpu name</t>
   </si>
@@ -282,6 +282,30 @@
   </si>
   <si>
     <t>11.30" (287mm)</t>
+  </si>
+  <si>
+    <t>Asus Radeon R9 290X 4GB Video Card</t>
+  </si>
+  <si>
+    <t>R9290X-4GD5</t>
+  </si>
+  <si>
+    <t>Sapphire Radeon R9 290 4GB Vapor-X Video Card</t>
+  </si>
+  <si>
+    <t>4.8 Average</t>
+  </si>
+  <si>
+    <t>Sapphire</t>
+  </si>
+  <si>
+    <t>100362VXSR</t>
+  </si>
+  <si>
+    <t>Radeon R9 290</t>
+  </si>
+  <si>
+    <t>1.03Ghz</t>
   </si>
 </sst>
 </file>
@@ -618,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V10"/>
+  <dimension ref="B1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,6 +1323,136 @@
         <v>481.92</v>
       </c>
     </row>
+    <row r="11" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4">
+        <v>1</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11" s="3">
+        <v>434.11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>2</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4">
+        <v>1</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="V12" s="3">
+        <v>424.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>